<commit_message>
Keep it simple, keep it stupid.
+ template for new vs 2008 project

Signed-off-by: Jinfeng Zhuang <Jinfengz@v-silicon.com>
</commit_message>
<xml_diff>
--- a/Documentation/VideoCodec_History.xlsx
+++ b/Documentation/VideoCodec_History.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github\ZSTACK\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8955250-271D-4E67-A67C-D0164869D4B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F24429D-65B8-461B-BDED-169BC452AABB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{49E42CD8-8C7C-4A5C-A95D-29B944C72FF5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="127">
   <si>
     <t>DCT</t>
   </si>
@@ -505,11 +505,21 @@
     <t>Joint Photographic Experts Group</t>
   </si>
   <si>
-    <t>Firsh puublished JPEG standard</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>CCITT became ITU-T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H.26x</t>
+  </si>
+  <si>
+    <t>MPEG</t>
+  </si>
+  <si>
+    <t>MPEG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Firsh published JPEG standard</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -892,7 +902,7 @@
   <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -932,6 +942,9 @@
       <c r="A3">
         <v>1984</v>
       </c>
+      <c r="B3" t="s">
+        <v>123</v>
+      </c>
       <c r="D3" t="s">
         <v>69</v>
       </c>
@@ -943,6 +956,9 @@
       <c r="A4" s="1">
         <v>1988</v>
       </c>
+      <c r="B4" t="s">
+        <v>123</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
@@ -954,6 +970,9 @@
       <c r="A5">
         <v>1988</v>
       </c>
+      <c r="B5" t="s">
+        <v>125</v>
+      </c>
       <c r="D5" t="s">
         <v>2</v>
       </c>
@@ -982,6 +1001,9 @@
       <c r="A7">
         <v>1990</v>
       </c>
+      <c r="B7" t="s">
+        <v>124</v>
+      </c>
       <c r="D7" t="s">
         <v>6</v>
       </c>
@@ -1011,7 +1033,7 @@
         <v>67</v>
       </c>
       <c r="E9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1028,13 +1050,16 @@
         <v>121</v>
       </c>
       <c r="E10" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1993</v>
       </c>
+      <c r="B11" t="s">
+        <v>124</v>
+      </c>
       <c r="D11" t="s">
         <v>2</v>
       </c>
@@ -1046,6 +1071,9 @@
       <c r="A12">
         <v>1994</v>
       </c>
+      <c r="B12" t="s">
+        <v>124</v>
+      </c>
       <c r="D12" t="s">
         <v>7</v>
       </c>
@@ -1057,6 +1085,9 @@
       <c r="A13">
         <v>1995</v>
       </c>
+      <c r="B13" t="s">
+        <v>123</v>
+      </c>
       <c r="C13" t="s">
         <v>66</v>
       </c>
@@ -1071,6 +1102,9 @@
       <c r="A14">
         <v>1996</v>
       </c>
+      <c r="B14" t="s">
+        <v>124</v>
+      </c>
       <c r="D14" t="s">
         <v>7</v>
       </c>
@@ -1141,6 +1175,9 @@
       <c r="A19">
         <v>1998</v>
       </c>
+      <c r="B19" t="s">
+        <v>124</v>
+      </c>
       <c r="D19" t="s">
         <v>7</v>
       </c>
@@ -1152,6 +1189,9 @@
       <c r="A20">
         <v>1998</v>
       </c>
+      <c r="B20" t="s">
+        <v>124</v>
+      </c>
       <c r="D20" t="s">
         <v>15</v>
       </c>
@@ -1163,6 +1203,9 @@
       <c r="A21">
         <v>1999</v>
       </c>
+      <c r="B21" t="s">
+        <v>124</v>
+      </c>
       <c r="D21" t="s">
         <v>15</v>
       </c>
@@ -1191,6 +1234,9 @@
       <c r="A23">
         <v>2000</v>
       </c>
+      <c r="B23" t="s">
+        <v>124</v>
+      </c>
       <c r="D23" t="s">
         <v>7</v>
       </c>
@@ -1230,6 +1276,9 @@
       <c r="A26">
         <v>2001</v>
       </c>
+      <c r="B26" t="s">
+        <v>124</v>
+      </c>
       <c r="C26" t="s">
         <v>39</v>
       </c>
@@ -1275,6 +1324,9 @@
       <c r="A29">
         <v>2003</v>
       </c>
+      <c r="B29" t="s">
+        <v>124</v>
+      </c>
       <c r="D29" t="s">
         <v>15</v>
       </c>
@@ -1303,6 +1355,9 @@
       <c r="A31">
         <v>2003</v>
       </c>
+      <c r="B31" t="s">
+        <v>123</v>
+      </c>
       <c r="D31" t="s">
         <v>25</v>
       </c>
@@ -1345,6 +1400,9 @@
       <c r="A34">
         <v>2004</v>
       </c>
+      <c r="B34" t="s">
+        <v>123</v>
+      </c>
       <c r="D34" t="s">
         <v>19</v>
       </c>
@@ -1421,6 +1479,9 @@
       <c r="A39">
         <v>2007</v>
       </c>
+      <c r="B39" t="s">
+        <v>124</v>
+      </c>
       <c r="D39" t="s">
         <v>22</v>
       </c>
@@ -1466,6 +1527,9 @@
       <c r="A42">
         <v>2009</v>
       </c>
+      <c r="B42" t="s">
+        <v>124</v>
+      </c>
       <c r="D42" t="s">
         <v>21</v>
       </c>
@@ -1494,6 +1558,9 @@
       <c r="A44">
         <v>2010</v>
       </c>
+      <c r="B44" t="s">
+        <v>123</v>
+      </c>
       <c r="D44" t="s">
         <v>19</v>
       </c>
@@ -1555,6 +1622,9 @@
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2013</v>
+      </c>
+      <c r="B48" t="s">
+        <v>124</v>
       </c>
       <c r="D48" t="s">
         <v>7</v>

</xml_diff>